<commit_message>
Volledige data set met juiste namen
</commit_message>
<xml_diff>
--- a/Volledige_Data_Set.xlsx
+++ b/Volledige_Data_Set.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\Projects\Biomechanis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DACE44-D838-47B5-917D-B63A756C5285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E562045-A8D7-468A-9883-DA7F19BD19E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{569A95A3-47FE-42D6-A588-8CC2E9F95304}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{569A95A3-47FE-42D6-A588-8CC2E9F95304}"/>
   </bookViews>
   <sheets>
-    <sheet name="Elien Eigen 1" sheetId="32" r:id="rId1"/>
-    <sheet name="Elien Eigen 2" sheetId="33" r:id="rId2"/>
-    <sheet name="Elien Eigen 3" sheetId="34" r:id="rId3"/>
-    <sheet name="Elien Eigen 4" sheetId="35" r:id="rId4"/>
-    <sheet name="Elien Eigen 5" sheetId="36" r:id="rId5"/>
-    <sheet name="Elien Eigen 6" sheetId="37" r:id="rId6"/>
-    <sheet name="Elien_Circ1" sheetId="20" r:id="rId7"/>
-    <sheet name="Elien_Circ2" sheetId="21" r:id="rId8"/>
-    <sheet name="Elien_Circ3" sheetId="22" r:id="rId9"/>
-    <sheet name="Elien_Circ4" sheetId="23" r:id="rId10"/>
-    <sheet name="Elien_Circ5" sheetId="24" r:id="rId11"/>
-    <sheet name="Elien_Circ6" sheetId="25" r:id="rId12"/>
+    <sheet name="Elien_Eigen_1" sheetId="32" r:id="rId1"/>
+    <sheet name="Elien_Eigen_2" sheetId="33" r:id="rId2"/>
+    <sheet name="Elien_Eigen_3" sheetId="34" r:id="rId3"/>
+    <sheet name="Elien_Eigen_4" sheetId="35" r:id="rId4"/>
+    <sheet name="Elien_Eigen_5" sheetId="36" r:id="rId5"/>
+    <sheet name="Elien_Eigen_6" sheetId="37" r:id="rId6"/>
+    <sheet name="Elien_Circular_1" sheetId="20" r:id="rId7"/>
+    <sheet name="Elien_Circular_2" sheetId="21" r:id="rId8"/>
+    <sheet name="Elien_Circular_3" sheetId="22" r:id="rId9"/>
+    <sheet name="Elien_Circular_4" sheetId="23" r:id="rId10"/>
+    <sheet name="Elien_Circular_5" sheetId="24" r:id="rId11"/>
+    <sheet name="Elien_Circular_6" sheetId="25" r:id="rId12"/>
     <sheet name="Yenthe_Circ1" sheetId="26" r:id="rId13"/>
     <sheet name="Yenthe_Circ2" sheetId="27" r:id="rId14"/>
     <sheet name="Yenthe_Circ3" sheetId="28" r:id="rId15"/>
@@ -151,24 +151,6 @@
     <t>Ball speed</t>
   </si>
   <si>
-    <t>Elien_Circ1</t>
-  </si>
-  <si>
-    <t>Elien_Circ2</t>
-  </si>
-  <si>
-    <t>Elien_Circ3</t>
-  </si>
-  <si>
-    <t>Elien_Circ4</t>
-  </si>
-  <si>
-    <t>Elien_Circ5</t>
-  </si>
-  <si>
-    <t>Elien_Circ6</t>
-  </si>
-  <si>
     <t>Yenthe_Circ1</t>
   </si>
   <si>
@@ -203,6 +185,24 @@
   </si>
   <si>
     <t>Elien_Eigen_6</t>
+  </si>
+  <si>
+    <t>Elien_Circular_1</t>
+  </si>
+  <si>
+    <t>Elien_Circular_2</t>
+  </si>
+  <si>
+    <t>Elien_Circular_3</t>
+  </si>
+  <si>
+    <t>Elien_Circular_4</t>
+  </si>
+  <si>
+    <t>Elien_Circular_5</t>
+  </si>
+  <si>
+    <t>Elien_Circular_6</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>149.22999999999999</v>
@@ -2368,8 +2368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFC7F33-CC2F-4B12-83CD-5CE1AD72D051}">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>157.22999999999999</v>
@@ -4199,7 +4199,7 @@
   <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>160.03</v>
@@ -5901,7 +5901,7 @@
   <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5939,7 +5939,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>153.38</v>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>151.91999999999999</v>
@@ -8949,7 +8949,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>154.63999999999999</v>
@@ -10679,7 +10679,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>149.16999999999999</v>
@@ -12861,7 +12861,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>151.28</v>
@@ -14873,7 +14873,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>149.63</v>
@@ -17184,7 +17184,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>147.07</v>
@@ -21591,7 +21591,7 @@
   <dimension ref="A1:H141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21629,7 +21629,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>149.97</v>
@@ -41911,7 +41911,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>143.84</v>
@@ -54355,7 +54355,7 @@
   <dimension ref="A1:H136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54393,7 +54393,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>145.78</v>
@@ -56381,8 +56381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E5B841-2C26-4C54-8E2F-C11204EFB83C}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I37" sqref="I36:I37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56420,7 +56420,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>144.27000000000001</v>
@@ -57969,7 +57969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1540ABCB-B664-4880-B5B3-5B61A354C644}">
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -58008,7 +58008,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>140.32</v>
@@ -59667,7 +59667,7 @@
   <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59712,7 +59712,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>153.88999999999999</v>
@@ -61904,7 +61904,7 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -61947,7 +61947,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>168.43</v>
@@ -63204,7 +63204,7 @@
   <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63247,7 +63247,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>164</v>

</xml_diff>

<commit_message>
Yenthe _circluar name changed
</commit_message>
<xml_diff>
--- a/Volledige_Data_Set.xlsx
+++ b/Volledige_Data_Set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\Projects\Biomechanis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E562045-A8D7-468A-9883-DA7F19BD19E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE80A6F-A123-4A3D-8CDD-72D02677511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="9" xr2:uid="{569A95A3-47FE-42D6-A588-8CC2E9F95304}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="19" xr2:uid="{569A95A3-47FE-42D6-A588-8CC2E9F95304}"/>
   </bookViews>
   <sheets>
     <sheet name="Elien_Eigen_1" sheetId="32" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="Elien_Circular_4" sheetId="23" r:id="rId10"/>
     <sheet name="Elien_Circular_5" sheetId="24" r:id="rId11"/>
     <sheet name="Elien_Circular_6" sheetId="25" r:id="rId12"/>
-    <sheet name="Yenthe_Circ1" sheetId="26" r:id="rId13"/>
-    <sheet name="Yenthe_Circ2" sheetId="27" r:id="rId14"/>
-    <sheet name="Yenthe_Circ3" sheetId="28" r:id="rId15"/>
-    <sheet name="Yenthe_Circ4" sheetId="29" r:id="rId16"/>
-    <sheet name="Yenthe_Circ5" sheetId="30" r:id="rId17"/>
-    <sheet name="Yenthe_Circ6" sheetId="31" r:id="rId18"/>
+    <sheet name="Yenthe_Circular_1" sheetId="26" r:id="rId13"/>
+    <sheet name="Yenthe_Circular_2" sheetId="27" r:id="rId14"/>
+    <sheet name="Yenthe_Circular_3" sheetId="28" r:id="rId15"/>
+    <sheet name="Yenthe_Circular_4" sheetId="29" r:id="rId16"/>
+    <sheet name="Yenthe_Circular_5" sheetId="30" r:id="rId17"/>
+    <sheet name="Yenthe_Circular_6" sheetId="31" r:id="rId18"/>
     <sheet name="Elien_Arrow_1" sheetId="2" r:id="rId19"/>
     <sheet name="Elien_Arrow_2" sheetId="3" r:id="rId20"/>
     <sheet name="Elien_Arrow_3" sheetId="4" r:id="rId21"/>
@@ -151,24 +151,6 @@
     <t>Ball speed</t>
   </si>
   <si>
-    <t>Yenthe_Circ1</t>
-  </si>
-  <si>
-    <t>Yenthe_Circ2</t>
-  </si>
-  <si>
-    <t>Yenthe_Circ3</t>
-  </si>
-  <si>
-    <t>Yenthe_Circ4</t>
-  </si>
-  <si>
-    <t>Yenthe_Circ5</t>
-  </si>
-  <si>
-    <t>Yenthe_Circ6</t>
-  </si>
-  <si>
     <t>Elien_Eigen_1</t>
   </si>
   <si>
@@ -203,6 +185,24 @@
   </si>
   <si>
     <t>Elien_Circular_6</t>
+  </si>
+  <si>
+    <t>Yenthe_Circular_1</t>
+  </si>
+  <si>
+    <t>Yenthe_Circular_2</t>
+  </si>
+  <si>
+    <t>Yenthe_Circular_3</t>
+  </si>
+  <si>
+    <t>Yenthe_Circular_4</t>
+  </si>
+  <si>
+    <t>Yenthe_Circular_5</t>
+  </si>
+  <si>
+    <t>Yenthe_Circular_6</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>149.22999999999999</v>
@@ -2368,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFC7F33-CC2F-4B12-83CD-5CE1AD72D051}">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>157.22999999999999</v>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>160.03</v>
@@ -5939,7 +5939,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>153.38</v>
@@ -7495,7 +7495,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>151.91999999999999</v>
@@ -8911,7 +8911,7 @@
   <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8949,7 +8949,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>154.63999999999999</v>
@@ -10641,7 +10641,7 @@
   <dimension ref="A1:H149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10679,7 +10679,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>149.16999999999999</v>
@@ -12823,7 +12823,7 @@
   <dimension ref="A1:H136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12861,7 +12861,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>151.28</v>
@@ -14835,7 +14835,7 @@
   <dimension ref="A1:H158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14873,7 +14873,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>149.63</v>
@@ -17146,7 +17146,7 @@
   <dimension ref="A1:H160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17184,7 +17184,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>147.07</v>
@@ -19479,7 +19479,7 @@
   <dimension ref="A1:M217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21629,7 +21629,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>149.97</v>
@@ -23729,12 +23729,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3556CC-1F35-416E-8A64-A8EBD7455A24}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
@@ -41911,7 +41912,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>143.84</v>
@@ -54393,7 +54394,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>145.78</v>
@@ -56420,7 +56421,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>144.27000000000001</v>
@@ -58008,7 +58009,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>140.32</v>
@@ -59712,7 +59713,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>153.88999999999999</v>
@@ -61947,7 +61948,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>168.43</v>
@@ -63247,7 +63248,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>164</v>

</xml_diff>